<commit_message>
Update combined to Sept 2021 data. Redo Figure 3 to show individual flex accounts
</commit_message>
<xml_diff>
--- a/PreCompact/PrePostCompactWaterRights.xlsx
+++ b/PreCompact/PrePostCompactWaterRights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\PreCompact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB555B4-F25D-49F3-902D-5D0704E6BD27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2AE170-8C4D-43E0-9967-17D56981E585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>State</t>
   </si>
@@ -83,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -155,9 +155,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -166,7 +163,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,160 +483,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C662015A-9B1D-4685-9F27-C780AA843A24}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" customWidth="1"/>
     <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="6" max="6" width="35.1796875" customWidth="1"/>
+    <col min="7" max="7" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="8"/>
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.53849999999999998</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <f>B5</f>
         <v>0.53849999999999998</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <f>1-B5</f>
         <v>0.46150000000000002</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f>D5</f>
         <v>0.46150000000000002</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="4">
+        <f>SUM(B5,D5)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>0.54743299999999995</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <f>B6</f>
         <v>0.54743299999999995</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.05</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="4">
+        <f t="shared" ref="F6:F7" si="0">SUM(B6,D6)</f>
+        <v>0.59743299999999999</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>1.6</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>1.75</v>
       </c>
-      <c r="D7" s="6">
-        <f>2.5-B7</f>
+      <c r="D7" s="4">
+        <f>F7-C7</f>
+        <v>0.75</v>
+      </c>
+      <c r="E7" s="4">
+        <f>$F$7-B7</f>
         <v>0.89999999999999991</v>
       </c>
-      <c r="E7" s="6">
-        <f>2.5-C7</f>
-        <v>0.75</v>
-      </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <f>SUM(B5:B8)</f>
         <v>2.6859329999999999</v>
       </c>
-      <c r="C9" s="8">
-        <f t="shared" ref="C9:E9" si="0">SUM(C5:C8)</f>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9:E9" si="1">SUM(C5:C8)</f>
         <v>2.8359329999999998</v>
       </c>
-      <c r="D9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.4115</v>
-      </c>
-      <c r="E9" s="8">
-        <f t="shared" si="0"/>
-        <v>1.2815000000000001</v>
+      <c r="D9" s="7">
+        <f t="shared" si="1"/>
+        <v>1.2615000000000001</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>1.4315</v>
       </c>
       <c r="F9" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -646,7 +663,7 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Split Pre-Post excel file into min/max worksheets
</commit_message>
<xml_diff>
--- a/PreCompact/PrePostCompactWaterRights.xlsx
+++ b/PreCompact/PrePostCompactWaterRights.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20379"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\PreCompact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2AE170-8C4D-43E0-9967-17D56981E585}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCC07A7-784E-4A5D-BF0C-3627B228DA97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" activeTab="1" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MinValues" sheetId="1" r:id="rId1"/>
+    <sheet name="MaxValues" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>Pre-Compact Rights</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -57,18 +55,6 @@
     <t>Kristi Hansen, State Engineers Office</t>
   </si>
   <si>
-    <t>{Castle, 2019 #2810}</t>
-  </si>
-  <si>
-    <t>Post-Compact Rights</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
     <t>References</t>
   </si>
   <si>
@@ -76,6 +62,18 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Pre 1922</t>
+  </si>
+  <si>
+    <t>Post 1922</t>
+  </si>
+  <si>
+    <t>USBR, 2020</t>
+  </si>
+  <si>
+    <t>Castle and Fleck (2019)</t>
   </si>
 </sst>
 </file>
@@ -149,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -162,11 +160,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,188 +482,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C662015A-9B1D-4685-9F27-C780AA843A24}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" customWidth="1"/>
-    <col min="7" max="7" width="35.1796875" customWidth="1"/>
+    <col min="5" max="5" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="C4" s="4">
+        <f>1-B4</f>
+        <v>0.46150000000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <f>SUM(B4,C4)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>0.53849999999999998</v>
-      </c>
-      <c r="C5" s="4">
-        <f>B5</f>
-        <v>0.53849999999999998</v>
+        <v>0.54743299999999995</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.05</v>
       </c>
       <c r="D5" s="4">
-        <f>1-B5</f>
-        <v>0.46150000000000002</v>
-      </c>
-      <c r="E5" s="4">
-        <f>D5</f>
-        <v>0.46150000000000002</v>
-      </c>
-      <c r="F5" s="4">
-        <f>SUM(B5,D5)</f>
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
+        <f>SUM(B5,C5)</f>
+        <v>0.59743299999999999</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4">
-        <v>0.54743299999999995</v>
+      <c r="B6" s="5">
+        <v>1.6</v>
       </c>
       <c r="C6" s="4">
-        <f>B6</f>
-        <v>0.54743299999999995</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="E6" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" ref="F6:F7" si="0">SUM(B6,D6)</f>
-        <v>0.59743299999999999</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <f>D6-B6</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
-        <v>1.6</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9">
+        <f>SUM(B4:B7)</f>
+        <v>2.6859329999999999</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" ref="C8:D8" si="0">SUM(C4:C7)</f>
+        <v>1.4115</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>4.4974330000000009</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BAAC0F-B2EF-4929-90B1-BD1EFC7D3C0A}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="5" max="5" width="35.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.53849999999999998</v>
+      </c>
+      <c r="C4" s="4">
+        <f>1-B4</f>
+        <v>0.46150000000000002</v>
+      </c>
+      <c r="D4" s="4">
+        <f>SUM(B4,C4)</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.54743299999999995</v>
+      </c>
+      <c r="C5" s="5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D5" s="4">
+        <f>SUM(B5,C5)</f>
+        <v>0.6174329999999999</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
         <v>1.75</v>
       </c>
-      <c r="D7" s="4">
-        <f>F7-C7</f>
+      <c r="C6" s="4">
+        <f>D6-B6</f>
         <v>0.75</v>
       </c>
-      <c r="E7" s="4">
-        <f>$F$7-B7</f>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="D6" s="4">
         <v>2.5</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9">
+        <f>SUM(B4:B7)</f>
+        <v>2.8359329999999998</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" ref="C8:D8" si="0">SUM(C4:C7)</f>
+        <v>1.2815000000000001</v>
+      </c>
+      <c r="D8" s="9">
+        <f t="shared" si="0"/>
+        <v>4.5174330000000005</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="7">
-        <f>SUM(B5:B8)</f>
-        <v>2.6859329999999999</v>
-      </c>
-      <c r="C9" s="7">
-        <f t="shared" ref="C9:E9" si="1">SUM(C5:C8)</f>
-        <v>2.8359329999999998</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="1"/>
-        <v>1.2615000000000001</v>
-      </c>
-      <c r="E9" s="7">
-        <f t="shared" si="1"/>
-        <v>1.4315</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>15</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="G3:G4"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Multiple: Add Pre-1922 rights and more detail on how inflow split
Correct version numbers, Update Pre/Post Compact water rights.
</commit_message>
<xml_diff>
--- a/PreCompact/PrePostCompactWaterRights.xlsx
+++ b/PreCompact/PrePostCompactWaterRights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\PreCompact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCC07A7-784E-4A5D-BF0C-3627B228DA97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCFF513-98C2-4531-B2E8-38C171E57C81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" activeTab="1" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
   </bookViews>
   <sheets>
     <sheet name="MinValues" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>State</t>
   </si>
@@ -70,10 +70,16 @@
     <t>Post 1922</t>
   </si>
   <si>
-    <t>USBR, 2020</t>
-  </si>
-  <si>
     <t>Castle and Fleck (2019)</t>
+  </si>
+  <si>
+    <t>USBR (2020)</t>
+  </si>
+  <si>
+    <t>USBR. (2020). "Upper Colorado River Basin Consumptive Uses and Losses 2016 – 2020 Upper Colorado Region ", Department of Interior. https://www.usbr.gov/uc/DocLibrary/Reports/ConsumptiveUsesLosses/20210800-ProvisionalUpperColoradoRiverBasin2016-2020-CULReport-508-UCRO.pdf.</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -484,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C662015A-9B1D-4685-9F27-C780AA843A24}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -524,12 +530,11 @@
         <v>0.53849999999999998</v>
       </c>
       <c r="C4" s="4">
-        <f>1-B4</f>
-        <v>0.46150000000000002</v>
+        <f>D4-B4</f>
+        <v>0.4415</v>
       </c>
       <c r="D4" s="4">
-        <f>SUM(B4,C4)</f>
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -568,20 +573,24 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="5">
-        <v>0.4</v>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.41499999999999998</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -594,11 +603,11 @@
       </c>
       <c r="C8" s="9">
         <f t="shared" ref="C8:D8" si="0">SUM(C4:C7)</f>
-        <v>1.4115</v>
+        <v>1.3915</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>4.4974330000000009</v>
+        <v>4.4924330000000001</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -622,10 +631,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BAAC0F-B2EF-4929-90B1-BD1EFC7D3C0A}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,12 +673,11 @@
         <v>0.53849999999999998</v>
       </c>
       <c r="C4" s="4">
-        <f>1-B4</f>
-        <v>0.46150000000000002</v>
+        <f>D4-B4</f>
+        <v>0.44450000000000001</v>
       </c>
       <c r="D4" s="4">
-        <f>SUM(B4,C4)</f>
-        <v>1</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>7</v>
@@ -708,7 +716,7 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -717,10 +725,12 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="3"/>
+      <c r="D7" s="4">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
@@ -732,11 +742,11 @@
       </c>
       <c r="C8" s="9">
         <f t="shared" ref="C8:D8" si="0">SUM(C4:C7)</f>
-        <v>1.2815000000000001</v>
+        <v>1.2645</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="0"/>
-        <v>4.5174330000000005</v>
+        <v>4.5154329999999998</v>
       </c>
       <c r="E8" s="8"/>
     </row>
@@ -748,6 +758,11 @@
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retry Pre 1922 Upper Basin rights table
</commit_message>
<xml_diff>
--- a/PreCompact/PrePostCompactWaterRights.xlsx
+++ b/PreCompact/PrePostCompactWaterRights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\PreCompact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCFF513-98C2-4531-B2E8-38C171E57C81}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B360EAE4-4F58-4E3E-A7C5-E7F73D9D4789}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
   </bookViews>
@@ -153,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -173,6 +173,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,7 +494,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +509,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">

</xml_diff>